<commit_message>
Internship Project Main file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,33 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khush\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RPA\UI Path Projects\SavingsYogi\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989BA006-7A41-4D12-8F8F-F1BE225D3798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040EEF43-D19A-4908-85DF-6B0396DB6B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -44,156 +30,168 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Asset</t>
+  </si>
+  <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>MaxRetryNumber</t>
+  </si>
+  <si>
+    <t>ExScreenshotsFolderPath</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_Success</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException</t>
+  </si>
+  <si>
+    <t>Business rule exception.</t>
+  </si>
+  <si>
+    <t>LogMessage_ApplicationException</t>
+  </si>
+  <si>
+    <t>System exception.</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
     <t>ProcessABCQueue</t>
   </si>
   <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>System exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
     <t>PDFPath</t>
   </si>
   <si>
-    <t>C:\UiPath Projects\SavingsYogi_WebScrapper\Data\Output\PDF</t>
+    <t>SSPath</t>
+  </si>
+  <si>
+    <t>HTMLpath</t>
   </si>
   <si>
     <t>Path to save pdf</t>
   </si>
   <si>
-    <t>SSPath</t>
-  </si>
-  <si>
-    <t>C:\UiPath Projects\SavingsYogi_WebScrapper\Data\Output\Screenshots</t>
-  </si>
-  <si>
     <t>Path to save screenshot (business rule)</t>
   </si>
   <si>
-    <t>HTMLpath</t>
-  </si>
-  <si>
-    <t>C:\UiPath Projects\SavingsYogi_WebScrapper\Data\Output\Page</t>
-  </si>
-  <si>
     <t>Path to save html pages</t>
   </si>
   <si>
+    <t>F:\RPA\UI Path Projects\SavingsYogi\Data\Output\PDF</t>
+  </si>
+  <si>
+    <t>F:\RPA\UI Path Projects\SavingsYogi\Data\Output\Screenshots</t>
+  </si>
+  <si>
+    <t>F:\RPA\UI Path Projects\SavingsYogi\Data\Output\Page</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1khwJZXEMUQTvGGWF6m1hGG8ZEm1SFFkWFqRQzfFZw78/edit?usp=sharing</t>
+  </si>
+  <si>
     <t>SheetURL</t>
   </si>
   <si>
@@ -203,22 +201,10 @@
     <t>StatusColumn</t>
   </si>
   <si>
+    <t>I</t>
+  </si>
+  <si>
     <t>Status column alph</t>
-  </si>
-  <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/spreadsheets/d/1MpvMl8EGAfM-XrbgcsHueFiOcE1REKd3Hjv73dp2gDY/edit?gid=0#gid=0</t>
   </si>
 </sst>
 </file>
@@ -616,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -644,34 +630,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1678,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1698,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1726,67 +1712,67 @@
     </row>
     <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -1794,52 +1780,52 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1857,38 +1843,38 @@
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>50</v>
@@ -1896,24 +1882,24 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2906,13 +2892,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>

</xml_diff>